<commit_message>
'master: init commit Сб янв 16 15:30:12 MSK 2021'
</commit_message>
<xml_diff>
--- a/My/OLD/Лист Microsoft Excel.xlsx
+++ b/My/OLD/Лист Microsoft Excel.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Отлично</t>
   </si>
@@ -55,6 +57,48 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Сопровождение с помощью автоматированной системы</t>
+  </si>
+  <si>
+    <t>Время на создание новой документации</t>
+  </si>
+  <si>
+    <t>Время на редактирование уже существующей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 часа * 514 API методов = 1028 часов = 128 рабочих дня </t>
+  </si>
+  <si>
+    <t>Сопровождение документации в ручном режиме</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 час * 514 API методов = 514 часов = 64 рабочих дня </t>
+  </si>
+  <si>
+    <t>30 минут * 514 API методов = 154 часа = 19 рабочих дней</t>
+  </si>
+  <si>
+    <t>15 минут * 514 API методов = 77 часов = 9 рабочих дней</t>
+  </si>
+  <si>
+    <t>Параметр</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>request.url</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Путь (URL) до API метода на сервер</t>
   </si>
 </sst>
 </file>
@@ -78,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,25 +130,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -382,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K8:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+    <sheetView topLeftCell="E7" workbookViewId="0">
       <selection activeCell="M8" sqref="M8:N13"/>
     </sheetView>
   </sheetViews>
@@ -581,4 +639,97 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G2:I4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="7:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="7:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="7:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F3:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
'master: init commit Вс янв 17 13:43:53 MSK 2021'
</commit_message>
<xml_diff>
--- a/My/OLD/Лист Microsoft Excel.xlsx
+++ b/My/OLD/Лист Microsoft Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Отлично</t>
   </si>
@@ -99,19 +99,47 @@
   </si>
   <si>
     <t>Путь (URL) до API метода на сервер</t>
+  </si>
+  <si>
+    <t>Запрос</t>
+  </si>
+  <si>
+    <t>Период</t>
+  </si>
+  <si>
+    <t>Количество</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>документация api</t>
+  </si>
+  <si>
+    <t>api doc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="[$-419]mmmm\ yyyy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -145,11 +173,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -158,6 +262,30 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -173,6 +301,381 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Статистика запроса </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>«API»</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист3!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>api</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист3!$C$12:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>[$-419]mmmm\ yyyy;@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист3!$D$12:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>546682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>550925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>547302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>557672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E664-49EC-91B8-08D509ECC309}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист3!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>api</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист3!$C$12:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>[$-419]mmmm\ yyyy;@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист3!$D$12:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>546682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>550925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>547302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>557672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E664-49EC-91B8-08D509ECC309}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="311317000"/>
+        <c:axId val="311317328"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="311317000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-419]mmmm\ yyyy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="311317328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="311317328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="311317000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1033461</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -656,7 +1159,7 @@
     <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:9" ht="30" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
         <v>13</v>
@@ -694,20 +1197,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:H4"/>
+  <dimension ref="C3:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" customWidth="1"/>
+    <col min="13" max="13" width="43" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
@@ -718,7 +1228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
@@ -729,7 +1239,129 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" spans="3:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="7">
+        <v>557682</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="7">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="11">
+        <v>44075</v>
+      </c>
+      <c r="I11" s="11">
+        <v>44104</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="12">
+        <v>44075</v>
+      </c>
+      <c r="D12">
+        <v>546682</v>
+      </c>
+      <c r="E12">
+        <v>2554</v>
+      </c>
+      <c r="H12" s="11">
+        <v>44105</v>
+      </c>
+      <c r="I12" s="11">
+        <v>44135</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="12">
+        <v>44105</v>
+      </c>
+      <c r="D13">
+        <v>550925</v>
+      </c>
+      <c r="E13">
+        <v>2569</v>
+      </c>
+      <c r="H13" s="11">
+        <v>44136</v>
+      </c>
+      <c r="I13" s="11">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="12">
+        <v>44136</v>
+      </c>
+      <c r="D14">
+        <v>547302</v>
+      </c>
+      <c r="E14">
+        <v>2676</v>
+      </c>
+      <c r="H14" s="11">
+        <v>44166</v>
+      </c>
+      <c r="I14" s="11">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C15" s="12">
+        <v>44166</v>
+      </c>
+      <c r="D15">
+        <v>557672</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2864</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M6:M8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
'master: init commit Вс янв 17 22:19:54 MSK 2021'
</commit_message>
<xml_diff>
--- a/My/OLD/Лист Microsoft Excel.xlsx
+++ b/My/OLD/Лист Microsoft Excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Отлично</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>api doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -643,6 +646,1643 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Статистика запроса </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>«</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>документация </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>API»</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист3!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>документация api</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист3!$C$18:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>[$-419]mmmm\ yyyy;@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист3!$D$18:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3797-45FA-85DC-D362DBCFE27D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="394811784"/>
+        <c:axId val="394810144"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="394811784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-419]mmmm\ yyyy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394810144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="394810144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394811784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Статистика запроса «</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>API doc»</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист3!$D$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>api doc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист3!$C$24:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>[$-419]mmmm\ yyyy;@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист3!$D$24:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67BC-48E3-8C57-DDF30BC7BBAC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="160741160"/>
+        <c:axId val="160746080"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="160741160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-419]mmmm\ yyyy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160746080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="160746080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160741160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -670,6 +2310,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1033461</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -943,7 +2643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K8:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M8" sqref="M8:N13"/>
     </sheetView>
   </sheetViews>
@@ -1197,10 +2897,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:N15"/>
+  <dimension ref="C3:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,6 +3056,88 @@
         <v>2864</v>
       </c>
     </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
+        <v>44075</v>
+      </c>
+      <c r="D18">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="12">
+        <v>44105</v>
+      </c>
+      <c r="D19">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="12">
+        <v>44136</v>
+      </c>
+      <c r="D20">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C21" s="12">
+        <v>44166</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="12">
+        <v>44075</v>
+      </c>
+      <c r="D24">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="12">
+        <v>44105</v>
+      </c>
+      <c r="D25">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="12">
+        <v>44136</v>
+      </c>
+      <c r="D26">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="12">
+        <v>44166</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="M6:M8"/>

</xml_diff>